<commit_message>
+ Save answer reading start and end
</commit_message>
<xml_diff>
--- a/FAQsBrowser/Doc/Tracking.xlsx
+++ b/FAQsBrowser/Doc/Tracking.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="41720" yWindow="2760" windowWidth="20840" windowHeight="12620" tabRatio="500"/>
+    <workbookView xWindow="46420" yWindow="7220" windowWidth="20840" windowHeight="12620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Click</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>Tab created</t>
-  </si>
-  <si>
-    <t>not tracked</t>
   </si>
   <si>
     <t>logOpenAnswer</t>
@@ -92,6 +89,12 @@
   </si>
   <si>
     <t>hideSearchBar</t>
+  </si>
+  <si>
+    <t>same as click</t>
+  </si>
+  <si>
+    <t>in-page jumping is not tracked</t>
   </si>
 </sst>
 </file>
@@ -417,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -431,7 +434,7 @@
     <col min="4" max="4" width="24.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="27" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -443,7 +446,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -460,14 +463,16 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="G2" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="48" x14ac:dyDescent="0.3">
@@ -475,22 +480,19 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
@@ -502,14 +504,16 @@
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>13</v>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>